<commit_message>
include price in sales record
</commit_message>
<xml_diff>
--- a/management/src/main/resources/sales_records_template.xlsx
+++ b/management/src/main/resources/sales_records_template.xlsx
@@ -39,7 +39,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-jx:area(lastCell="K2")</t>
+jx:area(lastCell="L2")</t>
         </r>
       </text>
     </comment>
@@ -63,7 +63,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="records" var="record" lastCell="K2")</t>
+jx:each(items="records" var="record" lastCell="L2")</t>
         </r>
       </text>
     </comment>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>${record.region}</t>
   </si>
@@ -138,6 +138,12 @@
   </si>
   <si>
     <t>日期</t>
+  </si>
+  <si>
+    <t>价格</t>
+  </si>
+  <si>
+    <t>${record.price}</t>
   </si>
 </sst>
 </file>
@@ -514,18 +520,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="11" width="18.5703125" customWidth="1"/>
+    <col min="1" max="12" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -557,10 +563,13 @@
         <v>20</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -591,17 +600,20 @@
       <c r="J2" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I3" s="1"/>
-      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I4" s="1"/>
-      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Change the price label.
</commit_message>
<xml_diff>
--- a/management/src/main/resources/sales_records_template.xlsx
+++ b/management/src/main/resources/sales_records_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15990" windowHeight="3915"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16740" windowHeight="3660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -135,9 +135,6 @@
     <t>日期</t>
   </si>
   <si>
-    <t>价格</t>
-  </si>
-  <si>
     <t>${record.price}</t>
   </si>
   <si>
@@ -145,6 +142,9 @@
   </si>
   <si>
     <t>${record.managerFullName}</t>
+  </si>
+  <si>
+    <t>进院价格</t>
   </si>
 </sst>
 </file>
@@ -524,7 +524,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,7 +564,7 @@
         <v>18</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>19</v>
@@ -584,10 +584,10 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G2" t="s">
         <v>4</v>
@@ -602,7 +602,7 @@
         <v>7</v>
       </c>
       <c r="K2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>9</v>

</xml_diff>